<commit_message>
Commit all in /Documents and Essays/ from the end of the semester.
</commit_message>
<xml_diff>
--- a/Senior Design documents and essays/Timeline.xlsx
+++ b/Senior Design documents and essays/Timeline.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a22b347cee9d1214/Documents/Senior Design documents and essays/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CODE\StudentLoanCalculator\Senior Design documents and essays\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Task Name</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>month (concurrent)</t>
-  </si>
-  <si>
     <t>now</t>
   </si>
   <si>
@@ -183,13 +180,31 @@
   </si>
   <si>
     <t>Difficulty</t>
+  </si>
+  <si>
+    <t>4, 5</t>
+  </si>
+  <si>
+    <t>4, 5, 6</t>
+  </si>
+  <si>
+    <t>5, 9</t>
+  </si>
+  <si>
+    <t>11, 12</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>all prev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +215,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -226,11 +256,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,11 +497,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="374268136"/>
-        <c:axId val="374270096"/>
+        <c:axId val="264496472"/>
+        <c:axId val="264494904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="374268136"/>
+        <c:axId val="264496472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -504,7 +544,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374270096"/>
+        <c:crossAx val="264494904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -512,7 +552,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="374270096"/>
+        <c:axId val="264494904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,7 +603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374268136"/>
+        <c:crossAx val="264496472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1456,24 +1496,28 @@
   <dimension ref="A3:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>52</v>
+      <c r="C3" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>1</v>
@@ -1484,7 +1528,7 @@
       <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -1492,373 +1536,456 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="6">
+        <v>2</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="6">
+        <v>3</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="6">
+        <v>4</v>
+      </c>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4">
+        <v>4</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="6">
+        <v>4</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="6">
+        <v>5</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C4">
+      <c r="C13" s="4">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="4">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="4">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="D15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="6">
+        <v>11</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="4">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="4">
+        <v>6</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>15</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="B18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>18</v>
       </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>20</v>
       </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>22</v>
       </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>16</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>17</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>18</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>19</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>20</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>21</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>22</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>